<commit_message>
Rerun scripts for 2035 and 2040 EEJ run update
</commit_message>
<xml_diff>
--- a/utilities/PBA40/emissions/ModelRuns.xlsx
+++ b/utilities/PBA40/emissions/ModelRuns.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Application\Model One\RTP2017\Scenarios\ICF_DIR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzorn\Documents\travel-model-one-v05\utilities\PBA40\emissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -80,9 +80,6 @@
     <t>2035_06_694</t>
   </si>
   <si>
-    <t>2035_06_696</t>
-  </si>
-  <si>
     <t>2040_06_690</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>2040_06_694</t>
   </si>
   <si>
-    <t>2040_06_696</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -105,6 +99,12 @@
   </si>
   <si>
     <t>category</t>
+  </si>
+  <si>
+    <t>2040_06_697</t>
+  </si>
+  <si>
+    <t>2035_06_697</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -460,13 +460,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -606,7 +606,7 @@
         <v>2035</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -617,7 +617,7 @@
         <v>2040</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>5</v>
@@ -628,7 +628,7 @@
         <v>2040</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>7</v>
@@ -639,7 +639,7 @@
         <v>2040</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -650,7 +650,7 @@
         <v>2040</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>11</v>
@@ -661,7 +661,7 @@
         <v>2040</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Update paths for Plan Amendment
and Box Sync -> Box
</commit_message>
<xml_diff>
--- a/utilities/PBA40/emissions/ModelRuns.xlsx
+++ b/utilities/PBA40/emissions/ModelRuns.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzorn\Documents\travel-model-one-v05\utilities\PBA40\emissions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzorn\Documents\travel-model-one-master\utilities\PBA40\Emissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,9 +77,6 @@
     <t>2035_06_693</t>
   </si>
   <si>
-    <t>2035_06_694</t>
-  </si>
-  <si>
     <t>2040_06_690</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>2040_06_693</t>
   </si>
   <si>
-    <t>2040_06_694</t>
-  </si>
-  <si>
     <t>year</t>
   </si>
   <si>
@@ -105,6 +99,12 @@
   </si>
   <si>
     <t>2035_06_697</t>
+  </si>
+  <si>
+    <t>2040_06_694_Amd1</t>
+  </si>
+  <si>
+    <t>2035_06_694_Amd1</t>
   </si>
 </sst>
 </file>
@@ -447,26 +447,26 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -595,7 +595,7 @@
         <v>2035</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>11</v>
@@ -606,7 +606,7 @@
         <v>2035</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
@@ -617,7 +617,7 @@
         <v>2040</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>5</v>
@@ -628,7 +628,7 @@
         <v>2040</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>7</v>
@@ -639,7 +639,7 @@
         <v>2040</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -650,7 +650,7 @@
         <v>2040</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>11</v>
@@ -661,7 +661,7 @@
         <v>2040</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Update scripts/paths for IncrementalProgress off model calculators
</commit_message>
<xml_diff>
--- a/utilities/PBA40/emissions/ModelRuns.xlsx
+++ b/utilities/PBA40/emissions/ModelRuns.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzorn\Documents\travel-model-one-master\utilities\PBA40\Emissions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\travel-model-one-master\utilities\PBA40\Emissions\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F3771E-7138-4A2E-B95B-CD9F6DAF4E73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19650" windowHeight="12690"/>
+    <workbookView xWindow="12045" yWindow="2715" windowWidth="14430" windowHeight="10575" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RTP2017" sheetId="1" r:id="rId1"/>
+    <sheet name="RTP2021" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>2005_05_003</t>
   </si>
@@ -105,12 +107,36 @@
   </si>
   <si>
     <t>2035_06_694_Amd1</t>
+  </si>
+  <si>
+    <t>2035_TM151_IPA_loPop_loAOC_00</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>2035_TM151_IPA_loPop_hiAOC_00</t>
+  </si>
+  <si>
+    <t>2035_TM151_IPA_hiPop_loAOC_00</t>
+  </si>
+  <si>
+    <t>2035_TM151_IPA_hiPop_hiAOC_00</t>
+  </si>
+  <si>
+    <t>IP_hiAOC</t>
+  </si>
+  <si>
+    <t>IP_hiPop</t>
+  </si>
+  <si>
+    <t>IP_hiPop_hiAOC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -442,12 +468,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -670,4 +696,80 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170D2EFC-85A6-4F44-9439-D7E63C3E4D90}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2035</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2035</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2035</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2035</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>